<commit_message>
adding initial crop report summary md
</commit_message>
<xml_diff>
--- a/data-raw/crop_reports.xlsx
+++ b/data-raw/crop_reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/klamath/klamathAgData/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098AD56A-B141-E141-8C38-C272F466A830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D217E9-AC97-A24D-89FC-CA9E6D87FBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25760" yWindow="500" windowWidth="50880" windowHeight="19360" activeTab="1" xr2:uid="{1B09B5AE-9B4E-2540-A0D9-8AF8FCE3095B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13800" activeTab="2" xr2:uid="{1B09B5AE-9B4E-2540-A0D9-8AF8FCE3095B}"/>
   </bookViews>
   <sheets>
     <sheet name="crop_statistics" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
     <sheet name="number_of_farms_and_pop" sheetId="4" r:id="rId5"/>
     <sheet name="crop_production" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">acreage_summary!$A$1:$H$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="153">
   <si>
     <t>Category</t>
   </si>
@@ -424,6 +427,81 @@
   </si>
   <si>
     <t>Seeds</t>
+  </si>
+  <si>
+    <t>ACRES IRRIGATED (LINES 11 + 12)</t>
+  </si>
+  <si>
+    <t>TOTAL AREA IN IRRIGATION ROTATION (CULTIVATION) (LINES 13 + 14)</t>
+  </si>
+  <si>
+    <t>TOTAL AREA NOT IN IRRIGATION ROTATION (LINES 16 + 17)</t>
+  </si>
+  <si>
+    <t>TOTAL IRRIGABLE AREA FOR SERVICE (LINES 15 + 18 + 19)</t>
+  </si>
+  <si>
+    <t>TOTAL IRRIGABLE AREA (LINES 20 + 21)</t>
+  </si>
+  <si>
+    <t>CLASS 6 – TEMPORARILY IRRIGATED</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>GROSS CROP VALUE (FROM LINE 194)</t>
+  </si>
+  <si>
+    <t>ADDITIONAL REVENUE (22-30)</t>
+  </si>
+  <si>
+    <t>FEDERAL FSA PAYMENTS</t>
+  </si>
+  <si>
+    <t>SUGAR PROGRAM</t>
+  </si>
+  <si>
+    <t>TOTAL ADDITIONAL REVENUE (LINES 33 + 34)</t>
+  </si>
+  <si>
+    <t>TOTAL VALUE (GROSS CROP VALUE PLUS ADDITIONAL REVENUE – 31 + 35)</t>
+  </si>
+  <si>
+    <t>TOTAL IRRIGATED ACREAGE (FROM LINE 13)</t>
+  </si>
+  <si>
+    <t>AVERAGE VALUE PER IRRIGATED ACRE (LINE 36 / LINE 37)</t>
+  </si>
+  <si>
+    <t>FULL TIME FARMS (Est.)</t>
+  </si>
+  <si>
+    <t>PART TIME FARMS (Est.)</t>
+  </si>
+  <si>
+    <t>NON-AGRICULTURAL LANDS (ACRES FROM LINE 19)</t>
+  </si>
+  <si>
+    <t>TOTAL (ACRES FROM LINE 20)</t>
+  </si>
+  <si>
+    <t>PEAS GREEN (PROCESSING)</t>
+  </si>
+  <si>
+    <t>POTATOES CHIP</t>
+  </si>
+  <si>
+    <t>POTATOES FRESH</t>
+  </si>
+  <si>
+    <t>PLNT</t>
+  </si>
+  <si>
+    <t>FT²</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
 </sst>
 </file>
@@ -785,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FFABCD-945A-CA45-A43D-2DF892A32A80}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,8 +876,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2019</v>
+      <c r="B1" t="s">
+        <v>134</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1153,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4D91A1-4530-CE45-B4E8-FE55F027DBB1}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1163,8 +1241,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2019</v>
+      <c r="B1" t="s">
+        <v>134</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1306,10 +1384,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBEC8B7-4AEA-6C46-8994-85276059A5B6}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,7 +2359,7 @@
         <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="C43">
         <v>122351.53</v>
@@ -2514,17 +2593,315 @@
         <v>26</v>
       </c>
     </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>63563.03</v>
+      </c>
+      <c r="E54">
+        <v>63563.03</v>
+      </c>
+      <c r="F54" t="s">
+        <v>81</v>
+      </c>
+      <c r="G54">
+        <v>2017</v>
+      </c>
+      <c r="H54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>169.4</v>
+      </c>
+      <c r="E55">
+        <v>169.4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>81</v>
+      </c>
+      <c r="G55">
+        <v>2017</v>
+      </c>
+      <c r="H55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56">
+        <v>63732.43</v>
+      </c>
+      <c r="E56">
+        <v>63732.43</v>
+      </c>
+      <c r="F56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G56">
+        <v>2017</v>
+      </c>
+      <c r="H56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>79</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57">
+        <v>973</v>
+      </c>
+      <c r="E57">
+        <v>973</v>
+      </c>
+      <c r="F57" t="s">
+        <v>81</v>
+      </c>
+      <c r="G57">
+        <v>2017</v>
+      </c>
+      <c r="H57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58">
+        <v>64705.43</v>
+      </c>
+      <c r="E58">
+        <v>64705.43</v>
+      </c>
+      <c r="F58" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58">
+        <v>2017</v>
+      </c>
+      <c r="H58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>81</v>
+      </c>
+      <c r="G59">
+        <v>2017</v>
+      </c>
+      <c r="H59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+      <c r="G60">
+        <v>2017</v>
+      </c>
+      <c r="H60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>81</v>
+      </c>
+      <c r="G61">
+        <v>2017</v>
+      </c>
+      <c r="H61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62">
+        <v>1083</v>
+      </c>
+      <c r="E62">
+        <v>1083</v>
+      </c>
+      <c r="F62" t="s">
+        <v>81</v>
+      </c>
+      <c r="G62">
+        <v>2017</v>
+      </c>
+      <c r="H62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63">
+        <v>65788.429999999993</v>
+      </c>
+      <c r="E63">
+        <v>65788.429999999993</v>
+      </c>
+      <c r="F63" t="s">
+        <v>81</v>
+      </c>
+      <c r="G63">
+        <v>2017</v>
+      </c>
+      <c r="H63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>81</v>
+      </c>
+      <c r="G64">
+        <v>2017</v>
+      </c>
+      <c r="H64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65">
+        <v>65788.429999999993</v>
+      </c>
+      <c r="E65">
+        <v>65788.429999999993</v>
+      </c>
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+      <c r="G65">
+        <v>2017</v>
+      </c>
+      <c r="H65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" t="s">
+        <v>81</v>
+      </c>
+      <c r="G66">
+        <v>2017</v>
+      </c>
+      <c r="H66" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{2EBEC8B7-4AEA-6C46-8994-85276059A5B6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FBCFAB-AE5E-724C-BAD3-2EBB3920BFDF}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2967,6 +3344,118 @@
         <v>2018</v>
       </c>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34">
+        <v>84471546.75</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39">
+        <v>84471546.75</v>
+      </c>
+      <c r="E39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40">
+        <v>63732.43</v>
+      </c>
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41">
+        <v>1325.41</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2974,10 +3463,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C5FAAF-9C42-7146-89CF-CD546F801C8A}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3230,6 +3719,62 @@
         <v>2018</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18">
+        <v>290</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19">
+        <v>120</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20">
+        <v>1083</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21">
+        <v>65788.429999999993</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3237,10 +3782,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40720FFB-9A99-7949-8B75-22B8721A2274}">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+      <selection activeCell="N151" sqref="N151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7233,6 +7778,1056 @@
         <v>2018</v>
       </c>
     </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>88</v>
+      </c>
+      <c r="B130" t="s">
+        <v>47</v>
+      </c>
+      <c r="C130">
+        <v>7039</v>
+      </c>
+      <c r="D130" t="s">
+        <v>48</v>
+      </c>
+      <c r="E130">
+        <v>114.58</v>
+      </c>
+      <c r="F130">
+        <v>806552.08</v>
+      </c>
+      <c r="G130">
+        <v>4.08</v>
+      </c>
+      <c r="H130">
+        <v>467.5</v>
+      </c>
+      <c r="I130">
+        <v>3290732.5</v>
+      </c>
+      <c r="J130" t="s">
+        <v>81</v>
+      </c>
+      <c r="K130">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>88</v>
+      </c>
+      <c r="B131" t="s">
+        <v>49</v>
+      </c>
+      <c r="C131">
+        <v>6677.1</v>
+      </c>
+      <c r="D131" t="s">
+        <v>48</v>
+      </c>
+      <c r="E131">
+        <v>104.17</v>
+      </c>
+      <c r="F131">
+        <v>695529.17</v>
+      </c>
+      <c r="G131">
+        <v>3.6</v>
+      </c>
+      <c r="H131">
+        <v>375</v>
+      </c>
+      <c r="I131">
+        <v>2503905</v>
+      </c>
+      <c r="J131" t="s">
+        <v>81</v>
+      </c>
+      <c r="K131">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>88</v>
+      </c>
+      <c r="B132" t="s">
+        <v>50</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132" t="s">
+        <v>48</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132" t="s">
+        <v>81</v>
+      </c>
+      <c r="K132">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>88</v>
+      </c>
+      <c r="B133" t="s">
+        <v>51</v>
+      </c>
+      <c r="C133">
+        <v>148.69999999999999</v>
+      </c>
+      <c r="D133" t="s">
+        <v>48</v>
+      </c>
+      <c r="E133">
+        <v>131.25</v>
+      </c>
+      <c r="F133">
+        <v>19512.5</v>
+      </c>
+      <c r="G133">
+        <v>2.56</v>
+      </c>
+      <c r="H133">
+        <v>336</v>
+      </c>
+      <c r="I133">
+        <v>49952</v>
+      </c>
+      <c r="J133" t="s">
+        <v>81</v>
+      </c>
+      <c r="K133">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>88</v>
+      </c>
+      <c r="B134" t="s">
+        <v>52</v>
+      </c>
+      <c r="C134">
+        <v>8470.6</v>
+      </c>
+      <c r="D134" t="s">
+        <v>48</v>
+      </c>
+      <c r="E134">
+        <v>108.33</v>
+      </c>
+      <c r="F134">
+        <v>917646.53</v>
+      </c>
+      <c r="G134">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H134">
+        <v>552.5</v>
+      </c>
+      <c r="I134">
+        <v>4679997.29</v>
+      </c>
+      <c r="J134" t="s">
+        <v>81</v>
+      </c>
+      <c r="K134">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>88</v>
+      </c>
+      <c r="B135" t="s">
+        <v>53</v>
+      </c>
+      <c r="C135">
+        <v>971</v>
+      </c>
+      <c r="D135" t="s">
+        <v>48</v>
+      </c>
+      <c r="E135">
+        <v>83.33</v>
+      </c>
+      <c r="F135">
+        <v>80916.67</v>
+      </c>
+      <c r="G135">
+        <v>3.6</v>
+      </c>
+      <c r="H135">
+        <v>300</v>
+      </c>
+      <c r="I135">
+        <v>291300</v>
+      </c>
+      <c r="J135" t="s">
+        <v>81</v>
+      </c>
+      <c r="K135">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>89</v>
+      </c>
+      <c r="B136" t="s">
+        <v>54</v>
+      </c>
+      <c r="C136">
+        <v>22304.5</v>
+      </c>
+      <c r="D136" t="s">
+        <v>55</v>
+      </c>
+      <c r="E136">
+        <v>6.5</v>
+      </c>
+      <c r="F136">
+        <v>144979.25</v>
+      </c>
+      <c r="G136">
+        <v>170</v>
+      </c>
+      <c r="H136">
+        <v>1105</v>
+      </c>
+      <c r="I136">
+        <v>24646472.5</v>
+      </c>
+      <c r="J136" t="s">
+        <v>81</v>
+      </c>
+      <c r="K136">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>89</v>
+      </c>
+      <c r="B137" t="s">
+        <v>56</v>
+      </c>
+      <c r="C137">
+        <v>2630</v>
+      </c>
+      <c r="D137" t="s">
+        <v>55</v>
+      </c>
+      <c r="E137">
+        <v>4.5</v>
+      </c>
+      <c r="F137">
+        <v>11835</v>
+      </c>
+      <c r="G137">
+        <v>184</v>
+      </c>
+      <c r="H137">
+        <v>828</v>
+      </c>
+      <c r="I137">
+        <v>2177640</v>
+      </c>
+      <c r="J137" t="s">
+        <v>81</v>
+      </c>
+      <c r="K137">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>89</v>
+      </c>
+      <c r="B138" t="s">
+        <v>57</v>
+      </c>
+      <c r="C138">
+        <v>2435</v>
+      </c>
+      <c r="D138" t="s">
+        <v>58</v>
+      </c>
+      <c r="E138">
+        <v>5</v>
+      </c>
+      <c r="F138">
+        <v>12175.08</v>
+      </c>
+      <c r="G138">
+        <v>15</v>
+      </c>
+      <c r="H138">
+        <v>75</v>
+      </c>
+      <c r="I138">
+        <v>182626.13</v>
+      </c>
+      <c r="J138" t="s">
+        <v>81</v>
+      </c>
+      <c r="K138">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>89</v>
+      </c>
+      <c r="B139" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139" t="s">
+        <v>55</v>
+      </c>
+      <c r="E139">
+        <v>145</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>10</v>
+      </c>
+      <c r="H139">
+        <v>1450</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139" t="s">
+        <v>81</v>
+      </c>
+      <c r="K139">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>89</v>
+      </c>
+      <c r="B140" t="s">
+        <v>60</v>
+      </c>
+      <c r="C140">
+        <v>30</v>
+      </c>
+      <c r="D140" t="s">
+        <v>55</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140" t="s">
+        <v>81</v>
+      </c>
+      <c r="K140">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>90</v>
+      </c>
+      <c r="B141" t="s">
+        <v>62</v>
+      </c>
+      <c r="C141">
+        <v>2209</v>
+      </c>
+      <c r="D141" t="s">
+        <v>63</v>
+      </c>
+      <c r="E141">
+        <v>90</v>
+      </c>
+      <c r="F141">
+        <v>198810</v>
+      </c>
+      <c r="G141">
+        <v>20</v>
+      </c>
+      <c r="H141">
+        <v>1800</v>
+      </c>
+      <c r="I141">
+        <v>3976200</v>
+      </c>
+      <c r="J141" t="s">
+        <v>81</v>
+      </c>
+      <c r="K141">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>90</v>
+      </c>
+      <c r="B142" t="s">
+        <v>64</v>
+      </c>
+      <c r="C142">
+        <v>443</v>
+      </c>
+      <c r="D142" t="s">
+        <v>55</v>
+      </c>
+      <c r="E142">
+        <v>2.5</v>
+      </c>
+      <c r="F142">
+        <v>1107.5</v>
+      </c>
+      <c r="G142">
+        <v>500</v>
+      </c>
+      <c r="H142">
+        <v>1250</v>
+      </c>
+      <c r="I142">
+        <v>553750</v>
+      </c>
+      <c r="J142" t="s">
+        <v>81</v>
+      </c>
+      <c r="K142">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>90</v>
+      </c>
+      <c r="B143" t="s">
+        <v>65</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143" t="s">
+        <v>63</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143" t="s">
+        <v>81</v>
+      </c>
+      <c r="K143">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>91</v>
+      </c>
+      <c r="B144" t="s">
+        <v>66</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144" t="s">
+        <v>67</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144" t="s">
+        <v>81</v>
+      </c>
+      <c r="K144">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>91</v>
+      </c>
+      <c r="B145" t="s">
+        <v>68</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145" t="s">
+        <v>63</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145" t="s">
+        <v>81</v>
+      </c>
+      <c r="K145">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>91</v>
+      </c>
+      <c r="B146" t="s">
+        <v>69</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146" t="s">
+        <v>67</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146" t="s">
+        <v>81</v>
+      </c>
+      <c r="K146">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>91</v>
+      </c>
+      <c r="B147" t="s">
+        <v>70</v>
+      </c>
+      <c r="C147">
+        <v>2286.1999999999998</v>
+      </c>
+      <c r="D147" t="s">
+        <v>67</v>
+      </c>
+      <c r="E147">
+        <v>460</v>
+      </c>
+      <c r="F147">
+        <v>1051644.33</v>
+      </c>
+      <c r="G147">
+        <v>7</v>
+      </c>
+      <c r="H147">
+        <v>3220</v>
+      </c>
+      <c r="I147">
+        <v>7361510.3300000001</v>
+      </c>
+      <c r="J147" t="s">
+        <v>81</v>
+      </c>
+      <c r="K147">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>91</v>
+      </c>
+      <c r="B148" t="s">
+        <v>147</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148" t="s">
+        <v>55</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>0</v>
+      </c>
+      <c r="J148" t="s">
+        <v>81</v>
+      </c>
+      <c r="K148">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>91</v>
+      </c>
+      <c r="B149" t="s">
+        <v>148</v>
+      </c>
+      <c r="C149">
+        <v>3683</v>
+      </c>
+      <c r="D149" t="s">
+        <v>67</v>
+      </c>
+      <c r="E149">
+        <v>520</v>
+      </c>
+      <c r="F149">
+        <v>1915160</v>
+      </c>
+      <c r="G149">
+        <v>8.6</v>
+      </c>
+      <c r="H149">
+        <v>4472</v>
+      </c>
+      <c r="I149">
+        <v>16470376</v>
+      </c>
+      <c r="J149" t="s">
+        <v>81</v>
+      </c>
+      <c r="K149">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150" t="s">
+        <v>149</v>
+      </c>
+      <c r="C150">
+        <v>4020</v>
+      </c>
+      <c r="D150" t="s">
+        <v>67</v>
+      </c>
+      <c r="E150">
+        <v>463</v>
+      </c>
+      <c r="F150">
+        <v>1861260</v>
+      </c>
+      <c r="G150">
+        <v>9.75</v>
+      </c>
+      <c r="H150">
+        <v>4514.25</v>
+      </c>
+      <c r="I150">
+        <v>18147285</v>
+      </c>
+      <c r="J150" t="s">
+        <v>81</v>
+      </c>
+      <c r="K150">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>91</v>
+      </c>
+      <c r="B151" t="s">
+        <v>74</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151" t="s">
+        <v>55</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151" t="s">
+        <v>81</v>
+      </c>
+      <c r="K151">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>91</v>
+      </c>
+      <c r="B152" t="s">
+        <v>75</v>
+      </c>
+      <c r="C152">
+        <v>30</v>
+      </c>
+      <c r="D152" t="s">
+        <v>67</v>
+      </c>
+      <c r="E152">
+        <v>140</v>
+      </c>
+      <c r="F152">
+        <v>4200</v>
+      </c>
+      <c r="G152">
+        <v>20</v>
+      </c>
+      <c r="H152">
+        <v>2800</v>
+      </c>
+      <c r="I152">
+        <v>84000</v>
+      </c>
+      <c r="J152" t="s">
+        <v>81</v>
+      </c>
+      <c r="K152">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>101</v>
+      </c>
+      <c r="B153" t="s">
+        <v>92</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153" t="s">
+        <v>150</v>
+      </c>
+      <c r="E153">
+        <v>300000</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H153">
+        <v>24900</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153" t="s">
+        <v>81</v>
+      </c>
+      <c r="K153">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>101</v>
+      </c>
+      <c r="B154" t="s">
+        <v>93</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154" t="s">
+        <v>151</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154">
+        <v>0.3</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154" t="s">
+        <v>81</v>
+      </c>
+      <c r="K154">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>102</v>
+      </c>
+      <c r="B155" t="s">
+        <v>94</v>
+      </c>
+      <c r="C155">
+        <v>186</v>
+      </c>
+      <c r="D155" t="s">
+        <v>55</v>
+      </c>
+      <c r="E155">
+        <v>1.25</v>
+      </c>
+      <c r="F155">
+        <v>232.5</v>
+      </c>
+      <c r="G155">
+        <v>240</v>
+      </c>
+      <c r="H155">
+        <v>300</v>
+      </c>
+      <c r="I155">
+        <v>55800</v>
+      </c>
+      <c r="J155" t="s">
+        <v>81</v>
+      </c>
+      <c r="K155">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>102</v>
+      </c>
+      <c r="B156" t="s">
+        <v>95</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156" t="s">
+        <v>67</v>
+      </c>
+      <c r="E156">
+        <v>350</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <v>17</v>
+      </c>
+      <c r="H156">
+        <v>5950</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156" t="s">
+        <v>81</v>
+      </c>
+      <c r="K156">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>102</v>
+      </c>
+      <c r="B157" t="s">
+        <v>96</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157" t="s">
+        <v>63</v>
+      </c>
+      <c r="E157">
+        <v>400</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>1.25</v>
+      </c>
+      <c r="H157">
+        <v>500</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157" t="s">
+        <v>81</v>
+      </c>
+      <c r="K157">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>103</v>
+      </c>
+      <c r="B158" t="s">
+        <v>124</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158" t="s">
+        <v>152</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158" t="s">
+        <v>81</v>
+      </c>
+      <c r="K158">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>103</v>
+      </c>
+      <c r="B159" t="s">
+        <v>100</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159" t="s">
+        <v>152</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159" t="s">
+        <v>81</v>
+      </c>
+      <c r="K159">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>